<commit_message>
Json reporter- fixed, some refactoring
</commit_message>
<xml_diff>
--- a/AvalancheTester/AvalancheTester.Application/DailyTestReportsOutput.xlsx
+++ b/AvalancheTester/AvalancheTester.Application/DailyTestReportsOutput.xlsx
@@ -11,6 +11,9 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
@@ -79,7 +82,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -87,12 +90,41 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -387,11 +419,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="C12" sqref="C12:C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="A2:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,7 +436,7 @@
     <col min="6" max="6" width="69.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row spans="1:6" ht="15.75" x14ac:dyDescent="0.25" outlineLevel="0" r="1">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -424,7 +456,7 @@
         <v>5</v>
       </c>
     </row>
-    <row spans="1:6" ht="15.75" x14ac:dyDescent="0.25" outlineLevel="0" r="2">
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -432,35 +464,8 @@
       <c r="E2" s="1"/>
       <c r="F2" s="4"/>
     </row>
-    <row outlineLevel="0" r="3">
-      <c r="A3" s="0" t="inlineStr">
-        <is>
-          <t>Бай Иван Хижара</t>
-        </is>
-      </c>
-      <c r="B3" s="0" t="inlineStr">
-        <is>
-          <t>Рила</t>
-        </is>
-      </c>
-      <c r="C3" s="0" t="inlineStr">
-        <is>
-          <t>Маркуджиците</t>
-        </is>
-      </c>
-      <c r="D3" s="0">
-        <v>23.3999996185303</v>
-      </c>
-      <c r="E3" s="0" t="inlineStr">
-        <is>
-          <t>10.02.2015</t>
-        </is>
-      </c>
-      <c r="F3" s="0" t="inlineStr">
-        <is>
-          <t>Компресионен тест 3 повторения: Слой 163-120 см. – СТ1, СТ3...</t>
-        </is>
-      </c>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D3" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>